<commit_message>
tarea: Añadir archivo faltante
</commit_message>
<xml_diff>
--- a/Reto1/Proyección Poblacional cantonal 2010-2020_procesado.xlsx
+++ b/Reto1/Proyección Poblacional cantonal 2010-2020_procesado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q225"/>
+  <dimension ref="A1:R225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,12 +484,17 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>numero_autorizaciones</t>
+          <t>numero_vigente_consumo_humano</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>tasa_población_2020_autorizaciones</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>provincia</t>
         </is>
       </c>
     </row>
@@ -542,10 +547,15 @@
         <v>0.01961012678062641</v>
       </c>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>318498</v>
+        <v>1.569868570603269e-06</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -597,10 +607,17 @@
         <v>-0.001180669132421941</v>
       </c>
       <c r="P3" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>4345.666666666667</v>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -652,10 +669,15 @@
         <v>0.009923808411038038</v>
       </c>
       <c r="P4" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Q4" t="n">
-        <v>5456</v>
+        <v>4.072987943955686e-05</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -707,10 +729,15 @@
         <v>0.004135375622937243</v>
       </c>
       <c r="P5" t="n">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="Q5" t="n">
-        <v>163.1320754716981</v>
+        <v>0.0009831135785334259</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -762,10 +789,17 @@
         <v>0.009574020498841661</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>29214</v>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -817,10 +851,15 @@
         <v>0.0007024238942680006</v>
       </c>
       <c r="P7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>5292</v>
+        <v>9.44822373393802e-05</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -872,10 +911,15 @@
         <v>-0.0005033229902824621</v>
       </c>
       <c r="P8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q8" t="n">
-        <v>593.7142857142857</v>
+        <v>0.0004812319538017325</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -927,10 +971,15 @@
         <v>0.008862824216100695</v>
       </c>
       <c r="P9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="n">
-        <v>4187</v>
+        <v>4.776689754000478e-05</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -982,10 +1031,17 @@
         <v>0.008450052839696399</v>
       </c>
       <c r="P10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>30509</v>
+        <v>0</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1037,10 +1093,15 @@
         <v>0.01013642854905008</v>
       </c>
       <c r="P11" t="n">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="Q11" t="n">
-        <v>84.24489795918367</v>
+        <v>0.001937984496124031</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>AZUAY</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1094,7 +1155,16 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1147,7 +1217,16 @@
       <c r="P13" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1200,7 +1279,16 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1251,10 +1339,17 @@
         <v>0.00829638384563347</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>3859</v>
+        <v>0</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1308,7 +1403,16 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1359,10 +1463,15 @@
         <v>0.01285709366932659</v>
       </c>
       <c r="P17" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="Q17" t="n">
-        <v>5179.190476190476</v>
+        <v>3.6777212838925e-05</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>BOLIVAR</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1414,10 +1523,15 @@
         <v>-0.008176940708857539</v>
       </c>
       <c r="P18" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="Q18" t="n">
-        <v>1685</v>
+        <v>5.934718100890208e-05</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>BOLIVAR</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1469,10 +1583,15 @@
         <v>0.005259631184899405</v>
       </c>
       <c r="P19" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q19" t="n">
-        <v>3475.6</v>
+        <v>5.754402117619979e-05</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>BOLIVAR</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1524,10 +1643,17 @@
         <v>0.01092724190120289</v>
       </c>
       <c r="P20" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>7040.5</v>
+        <v>0</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1579,10 +1705,15 @@
         <v>0.00170606122452428</v>
       </c>
       <c r="P21" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="Q21" t="n">
-        <v>1160.16</v>
+        <v>0.0002068680182043856</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>BOLIVAR</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1634,10 +1765,15 @@
         <v>0.01874170624225877</v>
       </c>
       <c r="P22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q22" t="n">
-        <v>8214.5</v>
+        <v>6.086797735711242e-05</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>BOLIVAR</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1691,7 +1827,16 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1742,10 +1887,17 @@
         <v>0.0162848530281726</v>
       </c>
       <c r="P24" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>86276</v>
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1797,10 +1949,17 @@
         <v>0.008183100136085319</v>
       </c>
       <c r="P25" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>2967.625</v>
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1852,10 +2011,17 @@
         <v>0.00986872058276227</v>
       </c>
       <c r="P26" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>68747</v>
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1909,7 +2075,16 @@
       <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1962,7 +2137,16 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2015,7 +2199,16 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2068,7 +2261,16 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2119,10 +2321,15 @@
         <v>0.01284398906724056</v>
       </c>
       <c r="P31" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q31" t="n">
-        <v>9308.636363636364</v>
+        <v>3.906440744176962e-05</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>CARCHI</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -2174,10 +2381,17 @@
         <v>0.003419035332349107</v>
       </c>
       <c r="P32" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>3105.6</v>
+        <v>0</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -2229,10 +2443,15 @@
         <v>-0.001357291347059852</v>
       </c>
       <c r="P33" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="Q33" t="n">
-        <v>575.7083333333334</v>
+        <v>0.0003618730549323298</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>CARCHI</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -2284,10 +2503,17 @@
         <v>-0.006635305575952055</v>
       </c>
       <c r="P34" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>3989.666666666667</v>
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -2339,10 +2565,15 @@
         <v>0.00718257004050884</v>
       </c>
       <c r="P35" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="Q35" t="n">
-        <v>3422.9</v>
+        <v>2.921499313447661e-05</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>CARCHI</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -2394,10 +2625,17 @@
         <v>0.0117294562877958</v>
       </c>
       <c r="P36" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>8931</v>
+        <v>0</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2449,10 +2687,17 @@
         <v>0.01519404471668746</v>
       </c>
       <c r="P37" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>205624</v>
+        <v>0</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -2506,7 +2751,16 @@
       <c r="P38" t="n">
         <v>0</v>
       </c>
-      <c r="Q38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2559,7 +2813,16 @@
       <c r="P39" t="n">
         <v>0</v>
       </c>
-      <c r="Q39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2612,7 +2875,16 @@
       <c r="P40" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2663,10 +2935,17 @@
         <v>0.010401694347172</v>
       </c>
       <c r="P41" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>67100</v>
+        <v>0</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -2720,7 +2999,16 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2773,7 +3061,16 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
-      <c r="Q43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2824,10 +3121,15 @@
         <v>0.01208139285462999</v>
       </c>
       <c r="P44" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q44" t="n">
-        <v>37721.14285714286</v>
+        <v>7.574380415681998e-06</v>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>CHIMBORAZO</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -2881,7 +3183,16 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2934,7 +3245,16 @@
       <c r="P46" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2987,7 +3307,16 @@
       <c r="P47" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -3040,7 +3369,16 @@
       <c r="P48" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -3091,10 +3429,15 @@
         <v>0.02255004686875879</v>
       </c>
       <c r="P49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q49" t="n">
-        <v>19430.33333333333</v>
+        <v>1.715530699421866e-05</v>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>CHIMBORAZO</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -3146,10 +3489,17 @@
         <v>0.008385895560337153</v>
       </c>
       <c r="P50" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q50" t="n">
-        <v>48395</v>
+        <v>0</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -3203,7 +3553,16 @@
       <c r="P51" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -3256,7 +3615,16 @@
       <c r="P52" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -3309,7 +3677,16 @@
       <c r="P53" t="n">
         <v>0</v>
       </c>
-      <c r="Q53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3362,7 +3739,16 @@
       <c r="P54" t="n">
         <v>0</v>
       </c>
-      <c r="Q54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3415,7 +3801,16 @@
       <c r="P55" t="n">
         <v>0</v>
       </c>
-      <c r="Q55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3468,7 +3863,16 @@
       <c r="P56" t="n">
         <v>0</v>
       </c>
-      <c r="Q56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3521,7 +3925,16 @@
       <c r="P57" t="n">
         <v>0</v>
       </c>
-      <c r="Q57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3574,7 +3987,16 @@
       <c r="P58" t="n">
         <v>0</v>
       </c>
-      <c r="Q58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3627,7 +4049,16 @@
       <c r="P59" t="n">
         <v>0</v>
       </c>
-      <c r="Q59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3680,7 +4111,16 @@
       <c r="P60" t="n">
         <v>0</v>
       </c>
-      <c r="Q60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3733,7 +4173,16 @@
       <c r="P61" t="n">
         <v>0</v>
       </c>
-      <c r="Q61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3787,7 +4236,12 @@
         <v>1</v>
       </c>
       <c r="Q62" t="n">
-        <v>87723</v>
+        <v>1.139951894030072e-05</v>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>EL ORO</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -3841,7 +4295,16 @@
       <c r="P63" t="n">
         <v>0</v>
       </c>
-      <c r="Q63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3894,7 +4357,16 @@
       <c r="P64" t="n">
         <v>0</v>
       </c>
-      <c r="Q64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3947,7 +4419,16 @@
       <c r="P65" t="n">
         <v>0</v>
       </c>
-      <c r="Q65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -4000,7 +4481,16 @@
       <c r="P66" t="n">
         <v>0</v>
       </c>
-      <c r="Q66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -4053,7 +4543,16 @@
       <c r="P67" t="n">
         <v>0</v>
       </c>
-      <c r="Q67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -4104,10 +4603,15 @@
         <v>0.01098378694612798</v>
       </c>
       <c r="P68" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q68" t="n">
-        <v>72909</v>
+        <v>4.571909275032347e-06</v>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>ESMERALDAS</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -4161,7 +4665,16 @@
       <c r="P69" t="n">
         <v>0</v>
       </c>
-      <c r="Q69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -4212,10 +4725,17 @@
         <v>0.005200734946768893</v>
       </c>
       <c r="P70" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q70" t="n">
-        <v>10368.66666666667</v>
+        <v>0</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -4269,7 +4789,16 @@
       <c r="P71" t="n">
         <v>0</v>
       </c>
-      <c r="Q71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -4322,7 +4851,16 @@
       <c r="P72" t="n">
         <v>0</v>
       </c>
-      <c r="Q72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -4373,10 +4911,15 @@
         <v>0.02655730609755524</v>
       </c>
       <c r="P73" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q73" t="n">
-        <v>13873.75</v>
+        <v>1.801964140913596e-05</v>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>ESMERALDAS</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -4431,7 +4974,12 @@
         <v>1</v>
       </c>
       <c r="Q74" t="n">
-        <v>31475</v>
+        <v>3.177124702144559e-05</v>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>ESMERALDAS</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -4485,7 +5033,16 @@
       <c r="P75" t="n">
         <v>0</v>
       </c>
-      <c r="Q75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -4539,7 +5096,12 @@
         <v>1</v>
       </c>
       <c r="Q76" t="n">
-        <v>2723665</v>
+        <v>3.671523480310538e-07</v>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>GUAYAS</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -4593,7 +5155,16 @@
       <c r="P77" t="n">
         <v>0</v>
       </c>
-      <c r="Q77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -4647,7 +5218,12 @@
         <v>1</v>
       </c>
       <c r="Q78" t="n">
-        <v>26348</v>
+        <v>3.795354486109002e-05</v>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>GUAYAS</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -4701,7 +5277,16 @@
       <c r="P79" t="n">
         <v>0</v>
       </c>
-      <c r="Q79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -4754,7 +5339,16 @@
       <c r="P80" t="n">
         <v>0</v>
       </c>
-      <c r="Q80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -4807,7 +5401,16 @@
       <c r="P81" t="n">
         <v>0</v>
       </c>
-      <c r="Q81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -4860,7 +5463,16 @@
       <c r="P82" t="n">
         <v>0</v>
       </c>
-      <c r="Q82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -4913,7 +5525,16 @@
       <c r="P83" t="n">
         <v>0</v>
       </c>
-      <c r="Q83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -4966,7 +5587,16 @@
       <c r="P84" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -5019,7 +5649,16 @@
       <c r="P85" t="n">
         <v>0</v>
       </c>
-      <c r="Q85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -5072,7 +5711,16 @@
       <c r="P86" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -5125,7 +5773,16 @@
       <c r="P87" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -5179,7 +5836,12 @@
         <v>1</v>
       </c>
       <c r="Q88" t="n">
-        <v>18451</v>
+        <v>5.419760446588261e-05</v>
+      </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>GUAYAS</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -5233,7 +5895,16 @@
       <c r="P89" t="n">
         <v>0</v>
       </c>
-      <c r="Q89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -5286,7 +5957,16 @@
       <c r="P90" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -5339,7 +6019,16 @@
       <c r="P91" t="n">
         <v>0</v>
       </c>
-      <c r="Q91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -5392,7 +6081,16 @@
       <c r="P92" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -5445,7 +6143,16 @@
       <c r="P93" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -5498,7 +6205,16 @@
       <c r="P94" t="n">
         <v>0</v>
       </c>
-      <c r="Q94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -5551,7 +6267,16 @@
       <c r="P95" t="n">
         <v>0</v>
       </c>
-      <c r="Q95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -5602,10 +6327,17 @@
         <v>0.004752254508621379</v>
       </c>
       <c r="P96" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q96" t="n">
-        <v>13132</v>
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -5659,7 +6391,16 @@
       <c r="P97" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -5712,7 +6453,16 @@
       <c r="P98" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -5765,7 +6515,16 @@
       <c r="P99" t="n">
         <v>0</v>
       </c>
-      <c r="Q99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -5818,7 +6577,16 @@
       <c r="P100" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -5869,10 +6637,15 @@
         <v>0.01636530047987217</v>
       </c>
       <c r="P101" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q101" t="n">
-        <v>31592.71428571429</v>
+        <v>4.521838217672248e-06</v>
+      </c>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>IMBABURA</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -5926,7 +6699,16 @@
       <c r="P102" t="n">
         <v>0</v>
       </c>
-      <c r="Q102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -5977,10 +6759,15 @@
         <v>0.00578135032383884</v>
       </c>
       <c r="P103" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q103" t="n">
-        <v>6314.714285714285</v>
+        <v>2.262289889826482e-05</v>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>IMBABURA</t>
+        </is>
       </c>
     </row>
     <row r="104">
@@ -6032,10 +6819,15 @@
         <v>0.01450510193292336</v>
       </c>
       <c r="P104" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q104" t="n">
-        <v>31446.25</v>
+        <v>7.950073538180228e-06</v>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>IMBABURA</t>
+        </is>
       </c>
     </row>
     <row r="105">
@@ -6087,10 +6879,17 @@
         <v>-0.002181464285497104</v>
       </c>
       <c r="P105" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q105" t="n">
-        <v>13269</v>
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="106">
@@ -6144,7 +6943,16 @@
       <c r="P106" t="n">
         <v>0</v>
       </c>
-      <c r="Q106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -6195,10 +7003,15 @@
         <v>0.02092953059831886</v>
       </c>
       <c r="P107" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q107" t="n">
-        <v>39158.85714285714</v>
+        <v>1.09444314732664e-05</v>
+      </c>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>LOJA</t>
+        </is>
       </c>
     </row>
     <row r="108">
@@ -6252,7 +7065,16 @@
       <c r="P108" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -6305,7 +7127,16 @@
       <c r="P109" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -6358,7 +7189,16 @@
       <c r="P110" t="n">
         <v>0</v>
       </c>
-      <c r="Q110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -6411,7 +7251,16 @@
       <c r="P111" t="n">
         <v>0</v>
       </c>
-      <c r="Q111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -6464,7 +7313,16 @@
       <c r="P112" t="n">
         <v>0</v>
       </c>
-      <c r="Q112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -6517,7 +7375,16 @@
       <c r="P113" t="n">
         <v>0</v>
       </c>
-      <c r="Q113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -6570,7 +7437,16 @@
       <c r="P114" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -6623,7 +7499,16 @@
       <c r="P115" t="n">
         <v>0</v>
       </c>
-      <c r="Q115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -6676,7 +7561,16 @@
       <c r="P116" t="n">
         <v>0</v>
       </c>
-      <c r="Q116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -6727,10 +7621,15 @@
         <v>0.006219113503645434</v>
       </c>
       <c r="P117" t="n">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="Q117" t="n">
-        <v>389.6046511627907</v>
+        <v>0.0006864442189458605</v>
+      </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>LOJA</t>
+        </is>
       </c>
     </row>
     <row r="118">
@@ -6784,7 +7683,16 @@
       <c r="P118" t="n">
         <v>0</v>
       </c>
-      <c r="Q118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -6837,7 +7745,16 @@
       <c r="P119" t="n">
         <v>0</v>
       </c>
-      <c r="Q119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -6890,7 +7807,16 @@
       <c r="P120" t="n">
         <v>0</v>
       </c>
-      <c r="Q120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R120" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -6943,7 +7869,16 @@
       <c r="P121" t="n">
         <v>0</v>
       </c>
-      <c r="Q121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -6996,7 +7931,16 @@
       <c r="P122" t="n">
         <v>0</v>
       </c>
-      <c r="Q122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R122" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -7049,7 +7993,16 @@
       <c r="P123" t="n">
         <v>0</v>
       </c>
-      <c r="Q123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -7102,7 +8055,16 @@
       <c r="P124" t="n">
         <v>0</v>
       </c>
-      <c r="Q124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R124" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -7155,7 +8117,16 @@
       <c r="P125" t="n">
         <v>0</v>
       </c>
-      <c r="Q125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R125" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -7208,7 +8179,16 @@
       <c r="P126" t="n">
         <v>0</v>
       </c>
-      <c r="Q126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -7261,7 +8241,16 @@
       <c r="P127" t="n">
         <v>0</v>
       </c>
-      <c r="Q127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -7314,7 +8303,16 @@
       <c r="P128" t="n">
         <v>0</v>
       </c>
-      <c r="Q128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R128" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -7367,7 +8365,16 @@
       <c r="P129" t="n">
         <v>0</v>
       </c>
-      <c r="Q129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -7420,7 +8427,16 @@
       <c r="P130" t="n">
         <v>0</v>
       </c>
-      <c r="Q130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R130" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -7473,7 +8489,16 @@
       <c r="P131" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -7526,7 +8551,16 @@
       <c r="P132" t="n">
         <v>0</v>
       </c>
-      <c r="Q132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R132" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -7579,7 +8613,16 @@
       <c r="P133" t="n">
         <v>0</v>
       </c>
-      <c r="Q133" t="inlineStr"/>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R133" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -7632,7 +8675,16 @@
       <c r="P134" t="n">
         <v>0</v>
       </c>
-      <c r="Q134" t="inlineStr"/>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R134" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -7685,7 +8737,16 @@
       <c r="P135" t="n">
         <v>0</v>
       </c>
-      <c r="Q135" t="inlineStr"/>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R135" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -7738,7 +8799,16 @@
       <c r="P136" t="n">
         <v>0</v>
       </c>
-      <c r="Q136" t="inlineStr"/>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R136" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -7789,10 +8859,17 @@
         <v>0.003419035332349107</v>
       </c>
       <c r="P137" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q137" t="n">
-        <v>3105.6</v>
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R137" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="138">
@@ -7844,10 +8921,15 @@
         <v>-0.0005105455725056163</v>
       </c>
       <c r="P138" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="Q138" t="n">
-        <v>5458.416666666667</v>
+        <v>6.106776995771058e-05</v>
+      </c>
+      <c r="R138" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="139">
@@ -7901,7 +8983,16 @@
       <c r="P139" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr"/>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R139" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -7954,7 +9045,16 @@
       <c r="P140" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R140" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -8005,10 +9105,15 @@
         <v>0.0009355045942336382</v>
       </c>
       <c r="P141" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="Q141" t="n">
-        <v>2764.62962962963</v>
+        <v>8.038046754638622e-05</v>
+      </c>
+      <c r="R141" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="142">
@@ -8060,10 +9165,15 @@
         <v>-0.00483090982556289</v>
       </c>
       <c r="P142" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q142" t="n">
-        <v>2688.571428571428</v>
+        <v>0.0001062699256110521</v>
+      </c>
+      <c r="R142" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="143">
@@ -8117,7 +9227,16 @@
       <c r="P143" t="n">
         <v>0</v>
       </c>
-      <c r="Q143" t="inlineStr"/>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R143" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -8170,7 +9289,16 @@
       <c r="P144" t="n">
         <v>0</v>
       </c>
-      <c r="Q144" t="inlineStr"/>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R144" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -8224,7 +9352,12 @@
         <v>1</v>
       </c>
       <c r="Q145" t="n">
-        <v>37093</v>
+        <v>2.695926455126304e-05</v>
+      </c>
+      <c r="R145" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="146">
@@ -8276,10 +9409,17 @@
         <v>-0.006393482443314868</v>
       </c>
       <c r="P146" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q146" t="n">
-        <v>29599</v>
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R146" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="147">
@@ -8333,7 +9473,16 @@
       <c r="P147" t="n">
         <v>0</v>
       </c>
-      <c r="Q147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R147" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -8386,7 +9535,16 @@
       <c r="P148" t="n">
         <v>0</v>
       </c>
-      <c r="Q148" t="inlineStr"/>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R148" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -8437,10 +9595,15 @@
         <v>0.00507041076017527</v>
       </c>
       <c r="P149" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="Q149" t="n">
-        <v>4460.214285714285</v>
+        <v>3.202921064010378e-05</v>
+      </c>
+      <c r="R149" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="150">
@@ -8492,10 +9655,17 @@
         <v>0.006094348639509417</v>
       </c>
       <c r="P150" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q150" t="n">
-        <v>8459.4</v>
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R150" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="151">
@@ -8549,7 +9719,16 @@
       <c r="P151" t="n">
         <v>0</v>
       </c>
-      <c r="Q151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R151" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -8600,10 +9779,15 @@
         <v>0.01053948090951673</v>
       </c>
       <c r="P152" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q152" t="n">
-        <v>31720.5</v>
+        <v>1.576267713308428e-05</v>
+      </c>
+      <c r="R152" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="153">
@@ -8657,7 +9841,16 @@
       <c r="P153" t="n">
         <v>0</v>
       </c>
-      <c r="Q153" t="inlineStr"/>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R153" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -8708,10 +9901,15 @@
         <v>0.01559376957544438</v>
       </c>
       <c r="P154" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q154" t="n">
-        <v>6172</v>
+        <v>8.101101749837978e-05</v>
+      </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="155">
@@ -8765,7 +9963,16 @@
       <c r="P155" t="n">
         <v>0</v>
       </c>
-      <c r="Q155" t="inlineStr"/>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R155" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -8818,7 +10025,16 @@
       <c r="P156" t="n">
         <v>0</v>
       </c>
-      <c r="Q156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R156" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -8869,10 +10085,15 @@
         <v>0.008241865747273902</v>
       </c>
       <c r="P157" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q157" t="n">
-        <v>3542.714285714286</v>
+        <v>4.032420662123472e-05</v>
+      </c>
+      <c r="R157" t="inlineStr">
+        <is>
+          <t>MANABI</t>
+        </is>
       </c>
     </row>
     <row r="158">
@@ -8924,10 +10145,17 @@
         <v>0.03213518727596374</v>
       </c>
       <c r="P158" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q158" t="n">
-        <v>58281</v>
+        <v>0</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R158" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="159">
@@ -8979,10 +10207,17 @@
         <v>0.008992463958816189</v>
       </c>
       <c r="P159" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q159" t="n">
-        <v>19555</v>
+        <v>0</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R159" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="160">
@@ -9036,7 +10271,16 @@
       <c r="P160" t="n">
         <v>0</v>
       </c>
-      <c r="Q160" t="inlineStr"/>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R160" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -9089,7 +10333,16 @@
       <c r="P161" t="n">
         <v>0</v>
       </c>
-      <c r="Q161" t="inlineStr"/>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R161" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -9142,7 +10395,16 @@
       <c r="P162" t="n">
         <v>0</v>
       </c>
-      <c r="Q162" t="inlineStr"/>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R162" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -9195,7 +10457,16 @@
       <c r="P163" t="n">
         <v>0</v>
       </c>
-      <c r="Q163" t="inlineStr"/>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R163" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -9248,7 +10519,16 @@
       <c r="P164" t="n">
         <v>0</v>
       </c>
-      <c r="Q164" t="inlineStr"/>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R164" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -9301,7 +10581,16 @@
       <c r="P165" t="n">
         <v>0</v>
       </c>
-      <c r="Q165" t="inlineStr"/>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R165" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -9354,7 +10643,16 @@
       <c r="P166" t="n">
         <v>0</v>
       </c>
-      <c r="Q166" t="inlineStr"/>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R166" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -9407,7 +10705,16 @@
       <c r="P167" t="n">
         <v>0</v>
       </c>
-      <c r="Q167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R167" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -9460,7 +10767,16 @@
       <c r="P168" t="n">
         <v>0</v>
       </c>
-      <c r="Q168" t="inlineStr"/>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R168" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -9513,7 +10829,16 @@
       <c r="P169" t="n">
         <v>0</v>
       </c>
-      <c r="Q169" t="inlineStr"/>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R169" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -9564,10 +10889,15 @@
         <v>0.02350618794182402</v>
       </c>
       <c r="P170" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q170" t="n">
-        <v>26394</v>
+        <v>1.26291328837362e-05</v>
+      </c>
+      <c r="R170" t="inlineStr">
+        <is>
+          <t>NAPO</t>
+        </is>
       </c>
     </row>
     <row r="171">
@@ -9619,10 +10949,17 @@
         <v>0.02544079881859746</v>
       </c>
       <c r="P171" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q171" t="n">
-        <v>16534</v>
+        <v>0</v>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R171" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="172">
@@ -9674,10 +11011,17 @@
         <v>0.02130900159225946</v>
       </c>
       <c r="P172" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q172" t="n">
-        <v>10142</v>
+        <v>0</v>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R172" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="173">
@@ -9731,7 +11075,16 @@
       <c r="P173" t="n">
         <v>0</v>
       </c>
-      <c r="Q173" t="inlineStr"/>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R173" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -9782,10 +11135,17 @@
         <v>0.01660242661638436</v>
       </c>
       <c r="P174" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q174" t="n">
-        <v>1488.666666666667</v>
+        <v>0</v>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R174" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="175">
@@ -9839,7 +11199,16 @@
       <c r="P175" t="n">
         <v>0</v>
       </c>
-      <c r="Q175" t="inlineStr"/>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R175" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -9892,7 +11261,16 @@
       <c r="P176" t="n">
         <v>0</v>
       </c>
-      <c r="Q176" t="inlineStr"/>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R176" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -9943,10 +11321,17 @@
         <v>0.0116264787573005</v>
       </c>
       <c r="P177" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q177" t="n">
-        <v>4150</v>
+        <v>0</v>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R177" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="178">
@@ -10000,7 +11385,16 @@
       <c r="P178" t="n">
         <v>0</v>
       </c>
-      <c r="Q178" t="inlineStr"/>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R178" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -10051,10 +11445,15 @@
         <v>0.01832804023236798</v>
       </c>
       <c r="P179" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="Q179" t="n">
-        <v>84292.15151515152</v>
+        <v>2.516500152248259e-06</v>
+      </c>
+      <c r="R179" t="inlineStr">
+        <is>
+          <t>PICHINCHA</t>
+        </is>
       </c>
     </row>
     <row r="180">
@@ -10106,10 +11505,15 @@
         <v>0.01940043812960806</v>
       </c>
       <c r="P180" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="Q180" t="n">
-        <v>7690</v>
+        <v>1.857700167193015e-05</v>
+      </c>
+      <c r="R180" t="inlineStr">
+        <is>
+          <t>PICHINCHA</t>
+        </is>
       </c>
     </row>
     <row r="181">
@@ -10161,10 +11565,15 @@
         <v>0.02559547693606341</v>
       </c>
       <c r="P181" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="Q181" t="n">
-        <v>3605.566666666667</v>
+        <v>5.54697828358002e-05</v>
+      </c>
+      <c r="R181" t="inlineStr">
+        <is>
+          <t>PICHINCHA</t>
+        </is>
       </c>
     </row>
     <row r="182">
@@ -10216,10 +11625,15 @@
         <v>0.02355381005267478</v>
       </c>
       <c r="P182" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q182" t="n">
-        <v>7213.5</v>
+        <v>4.620965319655276e-05</v>
+      </c>
+      <c r="R182" t="inlineStr">
+        <is>
+          <t>PICHINCHA</t>
+        </is>
       </c>
     </row>
     <row r="183">
@@ -10271,10 +11685,15 @@
         <v>0.02676890220833095</v>
       </c>
       <c r="P183" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="Q183" t="n">
-        <v>7695.533333333334</v>
+        <v>2.598910190326856e-05</v>
+      </c>
+      <c r="R183" t="inlineStr">
+        <is>
+          <t>PICHINCHA</t>
+        </is>
       </c>
     </row>
     <row r="184">
@@ -10328,7 +11747,16 @@
       <c r="P184" t="n">
         <v>0</v>
       </c>
-      <c r="Q184" t="inlineStr"/>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R184" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -10381,7 +11809,16 @@
       <c r="P185" t="n">
         <v>0</v>
       </c>
-      <c r="Q185" t="inlineStr"/>
+      <c r="Q185" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R185" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -10434,7 +11871,16 @@
       <c r="P186" t="n">
         <v>0</v>
       </c>
-      <c r="Q186" t="inlineStr"/>
+      <c r="Q186" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R186" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -10487,7 +11933,16 @@
       <c r="P187" t="n">
         <v>0</v>
       </c>
-      <c r="Q187" t="inlineStr"/>
+      <c r="Q187" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R187" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -10540,7 +11995,16 @@
       <c r="P188" t="n">
         <v>0</v>
       </c>
-      <c r="Q188" t="inlineStr"/>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R188" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -10593,7 +12057,16 @@
       <c r="P189" t="n">
         <v>0</v>
       </c>
-      <c r="Q189" t="inlineStr"/>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R189" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -10646,7 +12119,16 @@
       <c r="P190" t="n">
         <v>0</v>
       </c>
-      <c r="Q190" t="inlineStr"/>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R190" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -10699,7 +12181,16 @@
       <c r="P191" t="n">
         <v>0</v>
       </c>
-      <c r="Q191" t="inlineStr"/>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R191" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -10752,7 +12243,16 @@
       <c r="P192" t="n">
         <v>0</v>
       </c>
-      <c r="Q192" t="inlineStr"/>
+      <c r="Q192" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R192" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -10805,7 +12305,16 @@
       <c r="P193" t="n">
         <v>0</v>
       </c>
-      <c r="Q193" t="inlineStr"/>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R193" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -10858,7 +12367,16 @@
       <c r="P194" t="n">
         <v>0</v>
       </c>
-      <c r="Q194" t="inlineStr"/>
+      <c r="Q194" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R194" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -10911,7 +12429,16 @@
       <c r="P195" t="n">
         <v>0</v>
       </c>
-      <c r="Q195" t="inlineStr"/>
+      <c r="Q195" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R195" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -10962,10 +12489,17 @@
         <v>0.0210450007865199</v>
       </c>
       <c r="P196" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q196" t="n">
-        <v>6552.2</v>
+        <v>0</v>
+      </c>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R196" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="197">
@@ -11017,10 +12551,17 @@
         <v>0.01126962280806387</v>
       </c>
       <c r="P197" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q197" t="n">
-        <v>10679</v>
+        <v>0</v>
+      </c>
+      <c r="Q197" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R197" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="198">
@@ -11072,10 +12613,17 @@
         <v>0.04073365584185575</v>
       </c>
       <c r="P198" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q198" t="n">
-        <v>4007</v>
+        <v>0</v>
+      </c>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R198" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="199">
@@ -11127,10 +12675,17 @@
         <v>0.01563101822092328</v>
       </c>
       <c r="P199" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q199" t="n">
-        <v>7121</v>
+        <v>0</v>
+      </c>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R199" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="200">
@@ -11182,10 +12737,17 @@
         <v>0.0315160297407616</v>
       </c>
       <c r="P200" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q200" t="n">
-        <v>26447</v>
+        <v>0</v>
+      </c>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R200" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="201">
@@ -11237,10 +12799,17 @@
         <v>0.01985058259011023</v>
       </c>
       <c r="P201" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q201" t="n">
-        <v>2736.25</v>
+        <v>0</v>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R201" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="202">
@@ -11292,10 +12861,17 @@
         <v>0.02094180179357647</v>
       </c>
       <c r="P202" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q202" t="n">
-        <v>2771</v>
+        <v>0</v>
+      </c>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R202" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="203">
@@ -11349,7 +12925,16 @@
       <c r="P203" t="n">
         <v>0</v>
       </c>
-      <c r="Q203" t="inlineStr"/>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R203" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -11400,10 +12985,17 @@
         <v>0.04160735710296617</v>
       </c>
       <c r="P204" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q204" t="n">
-        <v>1997.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="Q204" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R204" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="205">
@@ -11457,7 +13049,16 @@
       <c r="P205" t="n">
         <v>0</v>
       </c>
-      <c r="Q205" t="inlineStr"/>
+      <c r="Q205" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R205" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -11510,7 +13111,16 @@
       <c r="P206" t="n">
         <v>0</v>
       </c>
-      <c r="Q206" t="inlineStr"/>
+      <c r="Q206" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R206" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -11563,7 +13173,16 @@
       <c r="P207" t="n">
         <v>0</v>
       </c>
-      <c r="Q207" t="inlineStr"/>
+      <c r="Q207" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R207" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -11614,10 +13233,17 @@
         <v>0.02411087342357152</v>
       </c>
       <c r="P208" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q208" t="n">
-        <v>5979.7</v>
+        <v>0</v>
+      </c>
+      <c r="Q208" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R208" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="209">
@@ -11671,7 +13297,16 @@
       <c r="P209" t="n">
         <v>0</v>
       </c>
-      <c r="Q209" t="inlineStr"/>
+      <c r="Q209" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R209" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -11724,7 +13359,16 @@
       <c r="P210" t="n">
         <v>0</v>
       </c>
-      <c r="Q210" t="inlineStr"/>
+      <c r="Q210" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R210" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -11775,10 +13419,17 @@
         <v>0.02441580687287413</v>
       </c>
       <c r="P211" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q211" t="n">
-        <v>57949</v>
+        <v>0</v>
+      </c>
+      <c r="Q211" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R211" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="212">
@@ -11830,10 +13481,17 @@
         <v>0.008406378304228768</v>
       </c>
       <c r="P212" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q212" t="n">
-        <v>1270.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="Q212" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R212" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="213">
@@ -11885,10 +13543,17 @@
         <v>0.03406859101124069</v>
       </c>
       <c r="P213" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q213" t="n">
-        <v>15882</v>
+        <v>0</v>
+      </c>
+      <c r="Q213" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R213" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
       </c>
     </row>
     <row r="214">
@@ -11942,7 +13607,16 @@
       <c r="P214" t="n">
         <v>0</v>
       </c>
-      <c r="Q214" t="inlineStr"/>
+      <c r="Q214" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R214" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -11993,10 +13667,15 @@
         <v>0.02502839101594687</v>
       </c>
       <c r="P215" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q215" t="n">
-        <v>13396.85714285714</v>
+        <v>6.398089104054256e-05</v>
+      </c>
+      <c r="R215" t="inlineStr">
+        <is>
+          <t>ORELLANA</t>
+        </is>
       </c>
     </row>
     <row r="216">
@@ -12050,7 +13729,16 @@
       <c r="P216" t="n">
         <v>0</v>
       </c>
-      <c r="Q216" t="inlineStr"/>
+      <c r="Q216" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R216" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -12104,7 +13792,12 @@
         <v>8</v>
       </c>
       <c r="Q217" t="n">
-        <v>4919</v>
+        <v>0.0002032933523073795</v>
+      </c>
+      <c r="R217" t="inlineStr">
+        <is>
+          <t>ORELLANA</t>
+        </is>
       </c>
     </row>
     <row r="218">
@@ -12158,7 +13851,16 @@
       <c r="P218" t="n">
         <v>0</v>
       </c>
-      <c r="Q218" t="inlineStr"/>
+      <c r="Q218" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R218" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -12211,7 +13913,16 @@
       <c r="P219" t="n">
         <v>0</v>
       </c>
-      <c r="Q219" t="inlineStr"/>
+      <c r="Q219" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R219" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -12262,10 +13973,15 @@
         <v>0.02433012272385928</v>
       </c>
       <c r="P220" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q220" t="n">
-        <v>62940.33333333334</v>
+        <v>5.29602109934806e-06</v>
+      </c>
+      <c r="R220" t="inlineStr">
+        <is>
+          <t>SANTA ELENA</t>
+        </is>
       </c>
     </row>
     <row r="221">
@@ -12319,7 +14035,16 @@
       <c r="P221" t="n">
         <v>0</v>
       </c>
-      <c r="Q221" t="inlineStr"/>
+      <c r="Q221" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R221" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -12372,7 +14097,16 @@
       <c r="P222" t="n">
         <v>0</v>
       </c>
-      <c r="Q222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R222" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -12425,7 +14159,16 @@
       <c r="P223" t="n">
         <v>0</v>
       </c>
-      <c r="Q223" t="inlineStr"/>
+      <c r="Q223" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R223" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -12478,7 +14221,16 @@
       <c r="P224" t="n">
         <v>0</v>
       </c>
-      <c r="Q224" t="inlineStr"/>
+      <c r="Q224" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R224" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -12531,7 +14283,16 @@
       <c r="P225" t="n">
         <v>0</v>
       </c>
-      <c r="Q225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="R225" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>